<commit_message>
Add PI, Quote, and Production Order endpoints
</commit_message>
<xml_diff>
--- a/templates/quotation_template_no_discount.xlsx
+++ b/templates/quotation_template_no_discount.xlsx
@@ -71,7 +71,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -137,6 +137,13 @@
     <border>
       <left/>
       <right style="thin"/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="thin"/>
       <diagonal/>
@@ -549,7 +556,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N33"/>
+  <dimension ref="A1:N35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -754,76 +761,62 @@
           <t>{{Quote.Export_Route_Carrier__c}}</t>
         </is>
       </c>
-      <c r="D10" s="5" t="n"/>
-      <c r="E10" s="5" t="n"/>
-      <c r="F10" s="4" t="n"/>
-      <c r="G10" s="6" t="inlineStr">
-        <is>
-          <t>{{Quote.Incoterms__c}}</t>
-        </is>
-      </c>
-      <c r="H10" s="5" t="n"/>
-      <c r="I10" s="5" t="n"/>
-      <c r="J10" s="5" t="n"/>
-      <c r="K10" s="5" t="n"/>
-      <c r="L10" s="5" t="n"/>
-      <c r="M10" s="5" t="n"/>
-      <c r="N10" s="4" t="n"/>
+      <c r="D10" s="8" t="n"/>
+      <c r="E10" s="8" t="n"/>
+      <c r="F10" s="8" t="n"/>
+      <c r="G10" s="13" t="inlineStr">
+        <is>
+          <t>FREIGHT: {{#if Quote.Incoterms__c 'contains' 'FREIGHT'}}☑{{else}}☐{{/if}}
+PREPAID: {{#if Quote.Incoterms__c 'contains' 'PREPAID'}}☑{{else}}☐{{/if}}
+COLLECT: {{#if Quote.Incoterms__c 'contains' 'COLLECT'}}☑{{else}}☐{{/if}}</t>
+        </is>
+      </c>
+      <c r="H10" s="8" t="n"/>
+      <c r="I10" s="8" t="n"/>
+      <c r="J10" s="8" t="n"/>
+      <c r="K10" s="8" t="n"/>
+      <c r="L10" s="8" t="n"/>
+      <c r="M10" s="8" t="n"/>
+      <c r="N10" s="8" t="n"/>
     </row>
     <row r="11" ht="25" customHeight="1">
       <c r="A11" s="9" t="n"/>
       <c r="B11" s="10" t="n"/>
-      <c r="C11" s="3" t="inlineStr">
-        <is>
-          <t>PACKING:</t>
-        </is>
-      </c>
-      <c r="D11" s="5" t="n"/>
-      <c r="E11" s="5" t="n"/>
-      <c r="F11" s="4" t="n"/>
-      <c r="G11" s="3" t="inlineStr">
-        <is>
-          <t>SHIPPING SCHEDULE:</t>
-        </is>
-      </c>
-      <c r="H11" s="5" t="n"/>
-      <c r="I11" s="5" t="n"/>
-      <c r="J11" s="5" t="n"/>
-      <c r="K11" s="5" t="n"/>
-      <c r="L11" s="5" t="n"/>
-      <c r="M11" s="5" t="n"/>
-      <c r="N11" s="4" t="n"/>
+      <c r="C11" s="8" t="n"/>
+      <c r="D11" s="8" t="n"/>
+      <c r="E11" s="8" t="n"/>
+      <c r="F11" s="8" t="n"/>
+      <c r="G11" s="8" t="n"/>
+      <c r="H11" s="8" t="n"/>
+      <c r="I11" s="8" t="n"/>
+      <c r="J11" s="8" t="n"/>
+      <c r="K11" s="8" t="n"/>
+      <c r="L11" s="8" t="n"/>
+      <c r="M11" s="8" t="n"/>
+      <c r="N11" s="8" t="n"/>
     </row>
     <row r="12" ht="25" customHeight="1">
       <c r="A12" s="9" t="n"/>
       <c r="B12" s="10" t="n"/>
-      <c r="C12" s="6" t="inlineStr">
-        <is>
-          <t>{{Quote.Packing__c}}</t>
-        </is>
-      </c>
-      <c r="D12" s="5" t="n"/>
-      <c r="E12" s="5" t="n"/>
-      <c r="F12" s="4" t="n"/>
-      <c r="G12" s="6" t="inlineStr">
-        <is>
-          <t>{{Quote.Shipping_Schedule__c}}</t>
-        </is>
-      </c>
-      <c r="H12" s="5" t="n"/>
-      <c r="I12" s="5" t="n"/>
-      <c r="J12" s="5" t="n"/>
-      <c r="K12" s="5" t="n"/>
-      <c r="L12" s="5" t="n"/>
-      <c r="M12" s="5" t="n"/>
-      <c r="N12" s="4" t="n"/>
+      <c r="C12" s="8" t="n"/>
+      <c r="D12" s="8" t="n"/>
+      <c r="E12" s="8" t="n"/>
+      <c r="F12" s="8" t="n"/>
+      <c r="G12" s="8" t="n"/>
+      <c r="H12" s="8" t="n"/>
+      <c r="I12" s="8" t="n"/>
+      <c r="J12" s="8" t="n"/>
+      <c r="K12" s="8" t="n"/>
+      <c r="L12" s="8" t="n"/>
+      <c r="M12" s="8" t="n"/>
+      <c r="N12" s="8" t="n"/>
     </row>
     <row r="13" ht="25" customHeight="1">
       <c r="A13" s="9" t="n"/>
       <c r="B13" s="10" t="n"/>
       <c r="C13" s="3" t="inlineStr">
         <is>
-          <t>TERMS OF SALE:</t>
+          <t>PACKING:</t>
         </is>
       </c>
       <c r="D13" s="5" t="n"/>
@@ -831,7 +824,7 @@
       <c r="F13" s="4" t="n"/>
       <c r="G13" s="3" t="inlineStr">
         <is>
-          <t>TERMS OF PAYMENT:</t>
+          <t>SHIPPING SCHEDULE:</t>
         </is>
       </c>
       <c r="H13" s="5" t="n"/>
@@ -842,58 +835,74 @@
       <c r="M13" s="5" t="n"/>
       <c r="N13" s="4" t="n"/>
     </row>
-    <row r="14" ht="20" customHeight="1">
+    <row r="14" ht="45" customHeight="1">
       <c r="A14" s="9" t="n"/>
       <c r="B14" s="10" t="n"/>
-      <c r="C14" s="13" t="inlineStr">
+      <c r="C14" s="6" t="inlineStr">
+        <is>
+          <t>{{Quote.Packing__c}}</t>
+        </is>
+      </c>
+      <c r="D14" s="5" t="n"/>
+      <c r="E14" s="5" t="n"/>
+      <c r="F14" s="4" t="n"/>
+      <c r="G14" s="6" t="inlineStr">
+        <is>
+          <t>{{Quote.Shipping_Schedule__c}}</t>
+        </is>
+      </c>
+      <c r="H14" s="5" t="n"/>
+      <c r="I14" s="5" t="n"/>
+      <c r="J14" s="5" t="n"/>
+      <c r="K14" s="5" t="n"/>
+      <c r="L14" s="5" t="n"/>
+      <c r="M14" s="5" t="n"/>
+      <c r="N14" s="4" t="n"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="9" t="n"/>
+      <c r="B15" s="10" t="n"/>
+      <c r="C15" s="3" t="inlineStr">
+        <is>
+          <t>TERMS OF SALE:</t>
+        </is>
+      </c>
+      <c r="D15" s="5" t="n"/>
+      <c r="E15" s="5" t="n"/>
+      <c r="F15" s="4" t="n"/>
+      <c r="G15" s="3" t="inlineStr">
+        <is>
+          <t>TERMS OF PAYMENT:</t>
+        </is>
+      </c>
+      <c r="H15" s="5" t="n"/>
+      <c r="I15" s="5" t="n"/>
+      <c r="J15" s="5" t="n"/>
+      <c r="K15" s="5" t="n"/>
+      <c r="L15" s="5" t="n"/>
+      <c r="M15" s="5" t="n"/>
+      <c r="N15" s="4" t="n"/>
+    </row>
+    <row r="16" ht="20" customHeight="1">
+      <c r="A16" s="9" t="n"/>
+      <c r="B16" s="10" t="n"/>
+      <c r="C16" s="13" t="inlineStr">
         <is>
           <t>FOB : {{#if Quote.Terms_of_Sale__c '==' 'FOB'}}☑{{else}}☐{{/if}}
 C&amp;F : {{#if Quote.Terms_of_Sale__c '==' 'C&amp;F'}}☑{{else}}☐{{/if}}
 CIF : {{#if Quote.Terms_of_Sale__c '==' 'CIF'}}☑{{else}}☐{{/if}}</t>
         </is>
       </c>
-      <c r="D14" s="8" t="n"/>
-      <c r="E14" s="8" t="n"/>
-      <c r="F14" s="8" t="n"/>
-      <c r="G14" s="13" t="inlineStr">
+      <c r="D16" s="8" t="n"/>
+      <c r="E16" s="8" t="n"/>
+      <c r="F16" s="8" t="n"/>
+      <c r="G16" s="13" t="inlineStr">
         <is>
           <t>IRREVOCABLE LETTER OF CREDIT : {{#if Quote.Terms_of_Payment__c '==' 'IRREVOCABLE LETTER OF CREDIT'}}☑{{else}}☐{{/if}}
 T/T AT SIGHT DRAFT           : {{#if Quote.Terms_of_Payment__c '==' 'T/T AT SIGHT DRAFT'}}☑{{else}}☐{{/if}}
 CASH IN ADVANCE/WIRE TRANSFER: {{#if Quote.Terms_of_Payment__c '==' 'CASH IN ADVANCE/WIRE TRANSFER'}}☑{{else}}☐{{/if}}</t>
         </is>
       </c>
-      <c r="H14" s="8" t="n"/>
-      <c r="I14" s="8" t="n"/>
-      <c r="J14" s="8" t="n"/>
-      <c r="K14" s="8" t="n"/>
-      <c r="L14" s="8" t="n"/>
-      <c r="M14" s="8" t="n"/>
-      <c r="N14" s="8" t="n"/>
-    </row>
-    <row r="15" ht="20" customHeight="1">
-      <c r="A15" s="9" t="n"/>
-      <c r="B15" s="10" t="n"/>
-      <c r="C15" s="8" t="n"/>
-      <c r="D15" s="8" t="n"/>
-      <c r="E15" s="8" t="n"/>
-      <c r="F15" s="8" t="n"/>
-      <c r="G15" s="8" t="n"/>
-      <c r="H15" s="8" t="n"/>
-      <c r="I15" s="8" t="n"/>
-      <c r="J15" s="8" t="n"/>
-      <c r="K15" s="8" t="n"/>
-      <c r="L15" s="8" t="n"/>
-      <c r="M15" s="8" t="n"/>
-      <c r="N15" s="8" t="n"/>
-    </row>
-    <row r="16" ht="20" customHeight="1">
-      <c r="A16" s="11" t="n"/>
-      <c r="B16" s="12" t="n"/>
-      <c r="C16" s="8" t="n"/>
-      <c r="D16" s="8" t="n"/>
-      <c r="E16" s="8" t="n"/>
-      <c r="F16" s="8" t="n"/>
-      <c r="G16" s="8" t="n"/>
       <c r="H16" s="8" t="n"/>
       <c r="I16" s="8" t="n"/>
       <c r="J16" s="8" t="n"/>
@@ -902,18 +911,26 @@
       <c r="M16" s="8" t="n"/>
       <c r="N16" s="8" t="n"/>
     </row>
-    <row r="18">
-      <c r="A18" s="14" t="inlineStr">
-        <is>
-          <t>REMARK NUMBER ON DOCUMENTS :</t>
-        </is>
-      </c>
-      <c r="B18" s="8" t="n"/>
-      <c r="C18" s="14" t="inlineStr">
-        <is>
-          <t>BANK DETAIL: A PLUS MINERAL MATERIAL CORPORATION</t>
-        </is>
-      </c>
+    <row r="17" ht="20" customHeight="1">
+      <c r="A17" s="9" t="n"/>
+      <c r="B17" s="10" t="n"/>
+      <c r="C17" s="8" t="n"/>
+      <c r="D17" s="8" t="n"/>
+      <c r="E17" s="8" t="n"/>
+      <c r="F17" s="8" t="n"/>
+      <c r="G17" s="8" t="n"/>
+      <c r="H17" s="8" t="n"/>
+      <c r="I17" s="8" t="n"/>
+      <c r="J17" s="8" t="n"/>
+      <c r="K17" s="8" t="n"/>
+      <c r="L17" s="8" t="n"/>
+      <c r="M17" s="8" t="n"/>
+      <c r="N17" s="8" t="n"/>
+    </row>
+    <row r="18" ht="20" customHeight="1">
+      <c r="A18" s="11" t="n"/>
+      <c r="B18" s="12" t="n"/>
+      <c r="C18" s="8" t="n"/>
       <c r="D18" s="8" t="n"/>
       <c r="E18" s="8" t="n"/>
       <c r="F18" s="8" t="n"/>
@@ -926,289 +943,261 @@
       <c r="M18" s="8" t="n"/>
       <c r="N18" s="8" t="n"/>
     </row>
-    <row r="19" ht="40" customHeight="1">
-      <c r="A19" s="6" t="inlineStr">
+    <row r="20">
+      <c r="A20" s="14" t="inlineStr">
+        <is>
+          <t>REMARK NUMBER ON DOCUMENTS :</t>
+        </is>
+      </c>
+      <c r="B20" s="8" t="n"/>
+      <c r="C20" s="14" t="inlineStr">
+        <is>
+          <t>BANK DETAIL: A PLUS MINERAL MATERIAL CORPORATION</t>
+        </is>
+      </c>
+      <c r="D20" s="8" t="n"/>
+      <c r="E20" s="8" t="n"/>
+      <c r="F20" s="8" t="n"/>
+      <c r="G20" s="8" t="n"/>
+      <c r="H20" s="8" t="n"/>
+      <c r="I20" s="8" t="n"/>
+      <c r="J20" s="8" t="n"/>
+      <c r="K20" s="8" t="n"/>
+      <c r="L20" s="8" t="n"/>
+      <c r="M20" s="8" t="n"/>
+      <c r="N20" s="8" t="n"/>
+    </row>
+    <row r="21" ht="40" customHeight="1">
+      <c r="A21" s="6" t="inlineStr">
         <is>
           <t>{{Quote.REMARK_NUMBER_ON_DOCUMENTS__c}}</t>
         </is>
       </c>
-      <c r="B19" s="8" t="n"/>
-      <c r="C19" s="3" t="inlineStr">
+      <c r="B21" s="8" t="n"/>
+      <c r="C21" s="3" t="inlineStr">
         <is>
           <t>Account No: 018.137.261.4117 Bank for Foreign Trade of Viet Nam (Vietcombank), Nam Sai Gon branch
 Swift Code: BFTVVNVX018 ; Tel: 84.8.5413.5124 ; Fax: 84.8.5413.5127</t>
         </is>
       </c>
-      <c r="D19" s="8" t="n"/>
-      <c r="E19" s="8" t="n"/>
-      <c r="F19" s="8" t="n"/>
-      <c r="G19" s="8" t="n"/>
-      <c r="H19" s="8" t="n"/>
-      <c r="I19" s="8" t="n"/>
-      <c r="J19" s="8" t="n"/>
-      <c r="K19" s="8" t="n"/>
-      <c r="L19" s="8" t="n"/>
-      <c r="M19" s="8" t="n"/>
-      <c r="N19" s="8" t="n"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="15" t="inlineStr">
+      <c r="D21" s="8" t="n"/>
+      <c r="E21" s="8" t="n"/>
+      <c r="F21" s="8" t="n"/>
+      <c r="G21" s="8" t="n"/>
+      <c r="H21" s="8" t="n"/>
+      <c r="I21" s="8" t="n"/>
+      <c r="J21" s="8" t="n"/>
+      <c r="K21" s="8" t="n"/>
+      <c r="L21" s="8" t="n"/>
+      <c r="M21" s="8" t="n"/>
+      <c r="N21" s="8" t="n"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="15" t="inlineStr">
         <is>
           <t>ITEM NO.</t>
         </is>
       </c>
-      <c r="B21" s="15" t="inlineStr">
+      <c r="B23" s="15" t="inlineStr">
         <is>
           <t>PRODUCT DESCRIPTION</t>
         </is>
       </c>
-      <c r="C21" s="15" t="inlineStr">
+      <c r="C23" s="15" t="inlineStr">
         <is>
           <t>SIZE (cm)</t>
         </is>
       </c>
-      <c r="D21" s="15" t="n"/>
-      <c r="E21" s="15" t="n"/>
-      <c r="F21" s="15" t="inlineStr">
+      <c r="D23" s="15" t="n"/>
+      <c r="E23" s="15" t="n"/>
+      <c r="F23" s="15" t="inlineStr">
         <is>
           <t>QUANTITY</t>
         </is>
       </c>
-      <c r="G21" s="15" t="n"/>
-      <c r="H21" s="15" t="n"/>
-      <c r="I21" s="15" t="n"/>
-      <c r="J21" s="15" t="n"/>
-      <c r="K21" s="15" t="n"/>
-      <c r="L21" s="15" t="inlineStr">
+      <c r="G23" s="15" t="n"/>
+      <c r="H23" s="15" t="n"/>
+      <c r="I23" s="15" t="n"/>
+      <c r="J23" s="15" t="n"/>
+      <c r="K23" s="15" t="n"/>
+      <c r="L23" s="15" t="inlineStr">
         <is>
           <t>Unit Price (USD)</t>
         </is>
       </c>
-      <c r="M21" s="15" t="inlineStr">
+      <c r="M23" s="15" t="inlineStr">
         <is>
           <t>Total Price (USD)</t>
         </is>
       </c>
-      <c r="N21" s="15" t="inlineStr">
+      <c r="N23" s="15" t="inlineStr">
         <is>
           <t>Packing (Pcs/Crate)</t>
         </is>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" s="15" t="n"/>
-      <c r="B22" s="15" t="n"/>
-      <c r="C22" s="15" t="inlineStr">
+    <row r="24">
+      <c r="A24" s="15" t="n"/>
+      <c r="B24" s="15" t="n"/>
+      <c r="C24" s="15" t="inlineStr">
         <is>
           <t>L</t>
         </is>
       </c>
-      <c r="D22" s="15" t="inlineStr">
+      <c r="D24" s="15" t="inlineStr">
         <is>
           <t>W</t>
         </is>
       </c>
-      <c r="E22" s="15" t="inlineStr">
+      <c r="E24" s="15" t="inlineStr">
         <is>
           <t>H</t>
         </is>
       </c>
-      <c r="F22" s="15" t="inlineStr">
+      <c r="F24" s="15" t="inlineStr">
         <is>
           <t>PCS</t>
         </is>
       </c>
-      <c r="G22" s="15" t="inlineStr">
+      <c r="G24" s="15" t="inlineStr">
         <is>
           <t>m2</t>
         </is>
       </c>
-      <c r="H22" s="15" t="inlineStr">
+      <c r="H24" s="15" t="inlineStr">
         <is>
           <t>Crates</t>
         </is>
       </c>
-      <c r="I22" s="15" t="inlineStr">
+      <c r="I24" s="15" t="inlineStr">
         <is>
           <t>m3</t>
         </is>
       </c>
-      <c r="J22" s="15" t="inlineStr">
+      <c r="J24" s="15" t="inlineStr">
         <is>
           <t>Tons</t>
         </is>
       </c>
-      <c r="K22" s="15" t="inlineStr">
+      <c r="K24" s="15" t="inlineStr">
         <is>
           <t>Cont.</t>
         </is>
       </c>
-      <c r="L22" s="15" t="n"/>
-      <c r="M22" s="15" t="n"/>
-      <c r="N22" s="15" t="n"/>
-    </row>
-    <row r="23" ht="30" customHeight="1">
-      <c r="A23" s="16" t="inlineStr">
+      <c r="L24" s="15" t="n"/>
+      <c r="M24" s="15" t="n"/>
+      <c r="N24" s="15" t="n"/>
+    </row>
+    <row r="25" ht="30" customHeight="1">
+      <c r="A25" s="16" t="inlineStr">
         <is>
           <t>{{TableStart:GetQuoteLine}}{{Quote_Line_Item_Number_Quote__c}}</t>
         </is>
       </c>
-      <c r="B23" s="13" t="inlineStr">
+      <c r="B25" s="13" t="inlineStr">
         <is>
           <t>{{Product_Description__c}}</t>
         </is>
       </c>
-      <c r="C23" s="16" t="inlineStr">
+      <c r="C25" s="16" t="inlineStr">
         <is>
           <t>{{L_Quote__c}}</t>
         </is>
       </c>
-      <c r="D23" s="16" t="inlineStr">
+      <c r="D25" s="16" t="inlineStr">
         <is>
           <t>{{W_Quote__c}}</t>
         </is>
       </c>
-      <c r="E23" s="16" t="inlineStr">
+      <c r="E25" s="16" t="inlineStr">
         <is>
           <t>{{H_Quote__c}}</t>
         </is>
       </c>
-      <c r="F23" s="16" t="inlineStr">
+      <c r="F25" s="16" t="inlineStr">
         <is>
           <t>{{PCS_Quote__c}}</t>
         </is>
       </c>
-      <c r="G23" s="16" t="inlineStr">
+      <c r="G25" s="16" t="inlineStr">
         <is>
           <t>{{m2__c}}</t>
         </is>
       </c>
-      <c r="H23" s="16" t="inlineStr">
+      <c r="H25" s="16" t="inlineStr">
         <is>
           <t>{{Crates_Quote__c}}</t>
         </is>
       </c>
-      <c r="I23" s="16" t="inlineStr">
+      <c r="I25" s="16" t="inlineStr">
         <is>
           <t>{{m3__c}}</t>
         </is>
       </c>
-      <c r="J23" s="16" t="inlineStr">
+      <c r="J25" s="16" t="inlineStr">
         <is>
           <t>{{Tons__c}}</t>
         </is>
       </c>
-      <c r="K23" s="16" t="inlineStr">
+      <c r="K25" s="16" t="inlineStr">
         <is>
           <t>{{Cont__c}}</t>
         </is>
       </c>
-      <c r="L23" s="17" t="inlineStr">
+      <c r="L25" s="17" t="inlineStr">
         <is>
           <t>{{UnitPrice}} {{Charge_Unit_Quote__c}}</t>
         </is>
       </c>
-      <c r="M23" s="16" t="inlineStr">
+      <c r="M25" s="16" t="inlineStr">
         <is>
           <t>{{Total_Price_USD__c\# #,##0.##}}</t>
         </is>
       </c>
-      <c r="N23" s="16" t="inlineStr">
+      <c r="N25" s="16" t="inlineStr">
         <is>
           <t>{{Packing_Quote__c}} {{TableEnd:GetQuoteLine}}</t>
         </is>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="18" t="n"/>
-      <c r="B24" s="18" t="n"/>
-      <c r="C24" s="18" t="n"/>
-      <c r="D24" s="18" t="n"/>
-      <c r="E24" s="18" t="n"/>
-      <c r="F24" s="18" t="n"/>
-      <c r="G24" s="18" t="n"/>
-      <c r="H24" s="18" t="inlineStr">
+    <row r="26">
+      <c r="A26" s="18" t="n"/>
+      <c r="B26" s="18" t="n"/>
+      <c r="C26" s="18" t="n"/>
+      <c r="D26" s="18" t="n"/>
+      <c r="E26" s="18" t="n"/>
+      <c r="F26" s="18" t="n"/>
+      <c r="G26" s="18" t="n"/>
+      <c r="H26" s="18" t="inlineStr">
         <is>
           <t>{{Quote.Total_Crates__c}}</t>
         </is>
       </c>
-      <c r="I24" s="18" t="inlineStr">
+      <c r="I26" s="18" t="inlineStr">
         <is>
           <t>{{Quote.Total_m3__c}}</t>
         </is>
       </c>
-      <c r="J24" s="18" t="inlineStr">
+      <c r="J26" s="18" t="inlineStr">
         <is>
           <t>{{Quote.Total_Tons__c}}</t>
         </is>
       </c>
-      <c r="K24" s="18" t="inlineStr">
+      <c r="K26" s="18" t="inlineStr">
         <is>
           <t>{{Quote.Total_Conts__c}}</t>
         </is>
       </c>
-      <c r="L24" s="18" t="n"/>
-      <c r="M24" s="18" t="n"/>
-      <c r="N24" s="18" t="n"/>
-    </row>
-    <row r="25" ht="50" customHeight="1">
-      <c r="A25" s="3" t="inlineStr">
+      <c r="L26" s="18" t="n"/>
+      <c r="M26" s="18" t="n"/>
+      <c r="N26" s="18" t="n"/>
+    </row>
+    <row r="27" ht="50" customHeight="1">
+      <c r="A27" s="3" t="inlineStr">
         <is>
           <t>1. All prices quoted herein are US dollars.
 2. Prices quoted herein for merchandise only are valid for 180 days.
 3. Any changes in shipping costs or insurance rates are for account of the buyer.</t>
-        </is>
-      </c>
-      <c r="B25" s="8" t="n"/>
-      <c r="C25" s="8" t="n"/>
-      <c r="D25" s="8" t="n"/>
-      <c r="E25" s="8" t="n"/>
-      <c r="F25" s="8" t="n"/>
-      <c r="G25" s="8" t="n"/>
-      <c r="H25" s="8" t="n"/>
-      <c r="I25" s="8" t="n"/>
-      <c r="J25" s="8" t="n"/>
-      <c r="K25" s="18" t="inlineStr">
-        <is>
-          <t>SUBTOTAL</t>
-        </is>
-      </c>
-      <c r="L25" s="5" t="n"/>
-      <c r="M25" s="4" t="n"/>
-      <c r="N25" s="18" t="inlineStr">
-        <is>
-          <t>{{Quote.Sub_Total_USD__c\# #,##0.##}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="26" ht="50" customHeight="1">
-      <c r="A26" s="8" t="n"/>
-      <c r="B26" s="8" t="n"/>
-      <c r="C26" s="8" t="n"/>
-      <c r="D26" s="8" t="n"/>
-      <c r="E26" s="8" t="n"/>
-      <c r="F26" s="8" t="n"/>
-      <c r="G26" s="8" t="n"/>
-      <c r="H26" s="8" t="n"/>
-      <c r="I26" s="8" t="n"/>
-      <c r="J26" s="8" t="n"/>
-      <c r="K26" s="18" t="inlineStr">
-        <is>
-          <t>Fumigation</t>
-        </is>
-      </c>
-      <c r="L26" s="5" t="n"/>
-      <c r="M26" s="4" t="n"/>
-      <c r="N26" s="18" t="inlineStr">
-        <is>
-          <t>{{Quote.Fumigation__c}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="27" ht="30" customHeight="1">
-      <c r="A27" s="3" t="inlineStr">
-        <is>
-          <t>In words: {{Quote.In_words__c}}</t>
         </is>
       </c>
       <c r="B27" s="8" t="n"/>
@@ -1222,36 +1211,88 @@
       <c r="J27" s="8" t="n"/>
       <c r="K27" s="18" t="inlineStr">
         <is>
-          <t>TOTAL:</t>
+          <t>SUBTOTAL</t>
         </is>
       </c>
       <c r="L27" s="5" t="n"/>
       <c r="M27" s="4" t="n"/>
       <c r="N27" s="18" t="inlineStr">
         <is>
+          <t>{{Quote.Sub_Total_USD__c\# #,##0.##}}</t>
+        </is>
+      </c>
+    </row>
+    <row r="28" ht="50" customHeight="1">
+      <c r="A28" s="8" t="n"/>
+      <c r="B28" s="8" t="n"/>
+      <c r="C28" s="8" t="n"/>
+      <c r="D28" s="8" t="n"/>
+      <c r="E28" s="8" t="n"/>
+      <c r="F28" s="8" t="n"/>
+      <c r="G28" s="8" t="n"/>
+      <c r="H28" s="8" t="n"/>
+      <c r="I28" s="8" t="n"/>
+      <c r="J28" s="8" t="n"/>
+      <c r="K28" s="18" t="inlineStr">
+        <is>
+          <t>Fumigation</t>
+        </is>
+      </c>
+      <c r="L28" s="5" t="n"/>
+      <c r="M28" s="4" t="n"/>
+      <c r="N28" s="18" t="inlineStr">
+        <is>
+          <t>{{Quote.Fumigation__c}}</t>
+        </is>
+      </c>
+    </row>
+    <row r="29" ht="30" customHeight="1">
+      <c r="A29" s="3" t="inlineStr">
+        <is>
+          <t>In words: {{Quote.In_words__c}}</t>
+        </is>
+      </c>
+      <c r="B29" s="8" t="n"/>
+      <c r="C29" s="8" t="n"/>
+      <c r="D29" s="8" t="n"/>
+      <c r="E29" s="8" t="n"/>
+      <c r="F29" s="8" t="n"/>
+      <c r="G29" s="8" t="n"/>
+      <c r="H29" s="8" t="n"/>
+      <c r="I29" s="8" t="n"/>
+      <c r="J29" s="8" t="n"/>
+      <c r="K29" s="18" t="inlineStr">
+        <is>
+          <t>TOTAL:</t>
+        </is>
+      </c>
+      <c r="L29" s="5" t="n"/>
+      <c r="M29" s="4" t="n"/>
+      <c r="N29" s="18" t="inlineStr">
+        <is>
           <t>{{Quote.Total_Price_USD__c\# #,##0.##}}</t>
         </is>
       </c>
     </row>
-    <row r="29">
-      <c r="B29" s="19" t="inlineStr">
+    <row r="31">
+      <c r="B31" s="19" t="inlineStr">
         <is>
           <t>FOR AND ON BEHALF OF BUYER</t>
         </is>
       </c>
-      <c r="K29" s="19" t="inlineStr">
+      <c r="K31" s="19" t="inlineStr">
         <is>
           <t>FOR AND ON BEHALF OF SELLER</t>
         </is>
       </c>
     </row>
-    <row r="33">
-      <c r="B33" s="19" t="inlineStr">
+    <row r="35">
+      <c r="B35" s="19" t="inlineStr">
         <is>
           <t>A PLUS CORP</t>
         </is>
       </c>
-      <c r="K33" s="19" t="inlineStr">
+      <c r="K35" s="19" t="inlineStr">
         <is>
           <t>{{Quote.Account.Name}}</t>
         </is>
@@ -1259,56 +1300,56 @@
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="G12:N12"/>
     <mergeCell ref="C8:F8"/>
-    <mergeCell ref="G11:N11"/>
-    <mergeCell ref="A10:B16"/>
+    <mergeCell ref="G16:N18"/>
+    <mergeCell ref="A10:B18"/>
     <mergeCell ref="C7:F7"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="B31:F31"/>
     <mergeCell ref="K7:N7"/>
-    <mergeCell ref="N21:N22"/>
-    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C21:N21"/>
     <mergeCell ref="C13:F13"/>
+    <mergeCell ref="B23:B24"/>
     <mergeCell ref="K6:N6"/>
-    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="F23:K23"/>
     <mergeCell ref="K27:M27"/>
-    <mergeCell ref="A25:J26"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="A27:J28"/>
     <mergeCell ref="C6:F6"/>
     <mergeCell ref="A6:B8"/>
-    <mergeCell ref="G10:N10"/>
+    <mergeCell ref="C15:F15"/>
     <mergeCell ref="G13:N13"/>
     <mergeCell ref="C5:F5"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="K33:N33"/>
+    <mergeCell ref="G10:N12"/>
+    <mergeCell ref="L23:L24"/>
+    <mergeCell ref="N23:N24"/>
     <mergeCell ref="K5:N5"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="K28:M28"/>
     <mergeCell ref="G8:J8"/>
-    <mergeCell ref="C19:N19"/>
-    <mergeCell ref="K29:N29"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="G15:N15"/>
+    <mergeCell ref="K35:N35"/>
     <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A23:A24"/>
     <mergeCell ref="G7:J7"/>
-    <mergeCell ref="C14:F16"/>
-    <mergeCell ref="C18:N18"/>
-    <mergeCell ref="L21:L22"/>
-    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="G14:N14"/>
     <mergeCell ref="E3:J3"/>
-    <mergeCell ref="K25:M25"/>
+    <mergeCell ref="M23:M24"/>
+    <mergeCell ref="C10:F12"/>
     <mergeCell ref="G6:J6"/>
     <mergeCell ref="C9:F9"/>
-    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="K31:N31"/>
+    <mergeCell ref="K29:M29"/>
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="G14:N16"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="C16:F18"/>
     <mergeCell ref="K8:N8"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="K26:M26"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="G9:N9"/>
     <mergeCell ref="G5:J5"/>
-    <mergeCell ref="F21:K21"/>
+    <mergeCell ref="C20:N20"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>